<commit_message>
Some more untitled measurement
</commit_message>
<xml_diff>
--- a/Documents/Measurements.xlsx
+++ b/Documents/Measurements.xlsx
@@ -133,9 +133,6 @@
     <t>=</t>
   </si>
   <si>
-    <t>ms</t>
-  </si>
-  <si>
     <t>Pattern to Pattern</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>No Power Supply, Photovoltaic mode</t>
+  </si>
+  <si>
+    <t>us</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1634,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1644,7 +1644,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1">
         <v>4225</v>
@@ -1660,7 +1660,7 @@
         <v>236.68639053254438</v>
       </c>
       <c r="M1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1692,7 +1692,7 @@
         <v>16666.666666666668</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1718,7 +1718,7 @@
         <v>8333.3333333333339</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -1746,7 +1746,7 @@
         <v>1000000</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -1774,11 +1774,11 @@
         <v>36</v>
       </c>
       <c r="L5" s="17">
-        <f t="shared" ref="L5" si="1">1000*1000/I5</f>
+        <f t="shared" ref="L5:L6" si="1">1000*1000/I5</f>
         <v>1000000</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -1805,6 +1805,13 @@
         <v>23</v>
       </c>
       <c r="H6" s="10"/>
+      <c r="I6">
+        <v>1080</v>
+      </c>
+      <c r="L6" s="17">
+        <f t="shared" si="1"/>
+        <v>925.92592592592598</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
@@ -1833,7 +1840,7 @@
         <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K8" t="s">
         <v>36</v>
@@ -1861,7 +1868,7 @@
         <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K9" t="s">
         <v>36</v>
@@ -1893,7 +1900,7 @@
         <v>1.5</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K10" t="s">
         <v>36</v>
@@ -1934,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K11" t="s">
         <v>36</v>
@@ -1966,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K12" t="s">
         <v>36</v>
@@ -1992,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K13" t="s">
         <v>36</v>
@@ -2101,7 +2108,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>35</v>
@@ -2114,11 +2121,11 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>

</xml_diff>